<commit_message>
fix: filter unit kerja saat tambah dan edit pegawai
</commit_message>
<xml_diff>
--- a/public/assets/excel/template_data_nilai_kedisiplinan.xlsx
+++ b/public/assets/excel/template_data_nilai_kedisiplinan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\project\kinerjaku\public\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A93B76-AD3C-4C81-A633-734831F910EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CBDE8B-31C1-466F-AAEF-F1FD5C2C8504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8E9A788A-93FA-4A9C-9BBB-E2C7D2B24B28}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>nip</t>
   </si>
@@ -46,6 +46,21 @@
   </si>
   <si>
     <t>M. Irpandi</t>
+  </si>
+  <si>
+    <t>Haryo Suro Kuncoro</t>
+  </si>
+  <si>
+    <t>Muhammad Al-fatih Ritonga</t>
+  </si>
+  <si>
+    <t>Aditya Maulana</t>
+  </si>
+  <si>
+    <t>Ocha Sugiarto</t>
+  </si>
+  <si>
+    <t>Hafiizh Yaafi</t>
   </si>
 </sst>
 </file>
@@ -404,10 +419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9798187B-52D8-4E52-B71B-65B4F855B568}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -431,12 +446,67 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
-        <v>2020020005</v>
+        <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>7</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C4" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>12</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
         <v>100</v>
       </c>
     </row>

</xml_diff>